<commit_message>
homogenized D1S input library
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.laghi\Documents\GitHub\JADE\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0E8FE-73C1-4A33-A1EF-3EAF4F05C241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923DF637-8346-44B3-9C7B-1053A5FA24AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4404" yWindow="2580" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>xsdir Path</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>SphereSDDR.i</t>
+  </si>
+  <si>
+    <t>Frascati Neutron Generator SDDR experimen</t>
+  </si>
+  <si>
+    <t>FNG</t>
   </si>
 </sst>
 </file>
@@ -818,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1096,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,7 +1195,7 @@
         <v>34</v>
       </c>
       <c r="F4" s="12">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -1199,15 +1205,30 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
+      <c r="A5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="12">
+        <v>500000000</v>
+      </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>

</xml_diff>

<commit_message>
Independent folder location set up, default config changed for linux
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.laghi\Documents\GitHub\JADE\Code\default_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp30130\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4E80F9-4E8E-424E-A476-7457714694AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8E7FD6-501D-443D-BB4E-70EE003A2B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>ITER 1D (by M. Sawan)</t>
   </si>
   <si>
-    <t>C:\Documents\MCNP\MCNP_DATA\xsdir_mcnp6.2</t>
-  </si>
-  <si>
     <t>32c</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>Frascati Neutron Generator SDDR experiment</t>
+  </si>
+  <si>
+    <t>/home/mcnp/xs/xsdir_mcnp6.2</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,7 +449,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -747,31 +747,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1A2DE-3EB8-4AD4-9CF1-023800AFF144}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
     <col min="2" max="2" width="106" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18" hidden="1" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -779,7 +779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -787,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -795,7 +795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -803,7 +803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.600000000000001" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -824,25 +824,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" style="21" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="14" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" style="14" customWidth="1"/>
-    <col min="8" max="9" width="21.109375" style="14" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="19"/>
-    <col min="11" max="16384" width="8.88671875" style="14"/>
+    <col min="2" max="2" width="16.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="14" customWidth="1"/>
+    <col min="8" max="9" width="21.140625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="19"/>
+    <col min="11" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>29</v>
       </c>
@@ -856,7 +856,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -870,7 +870,7 @@
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>31</v>
       </c>
@@ -896,13 +896,13 @@
         <v>21</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>32</v>
       </c>
@@ -927,10 +927,10 @@
         <v>10</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>37</v>
       </c>
@@ -953,15 +953,15 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>35</v>
@@ -979,15 +979,15 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>35</v>
@@ -1005,15 +1005,15 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>49</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>35</v>
@@ -1031,15 +1031,15 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>51</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>35</v>
@@ -1057,15 +1057,15 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>35</v>
@@ -1085,7 +1085,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1106,19 +1106,19 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="9" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="9" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="26" t="s">
         <v>29</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="I1" s="26"/>
       <c r="J1" s="26"/>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>31</v>
       </c>
@@ -1172,18 +1172,18 @@
         <v>21</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>35</v>
@@ -1201,15 +1201,15 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>35</v>
@@ -1227,10 +1227,10 @@
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1241,7 +1241,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -1252,7 +1252,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1263,7 +1263,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1292,13 +1292,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1333,15 +1333,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1349,9 +1349,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Fixed up to SphereTest
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp59582\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp45674\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E31929D-8024-4ECA-B263-0EF29DE9A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1C24ED-8738-450F-9AF1-C27D6A00018C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>Default Benchmarks</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>/home/sbradnam/Projects/EPSRC/Benchmarking/software/freia/JADE/Configuration/openmc_config.sh</t>
+  </si>
+  <si>
+    <t>Custom Inputs</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -468,6 +471,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -486,10 +495,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -808,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1A2DE-3EB8-4AD4-9CF1-023800AFF144}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -819,10 +828,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -861,7 +870,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -869,38 +878,38 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="23"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="23"/>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="23">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="23" t="s">
         <v>46</v>
       </c>
     </row>
@@ -923,10 +932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,38 +945,40 @@
     <col min="3" max="3" width="13.140625" style="14" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9.42578125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="14" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="14"/>
+    <col min="8" max="9" width="16.28515625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="14" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
@@ -995,8 +1006,11 @@
       <c r="I3" s="17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>19</v>
       </c>
@@ -1024,8 +1038,9 @@
       <c r="I4" s="20">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="30"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>23</v>
       </c>
@@ -1053,8 +1068,9 @@
       <c r="I5" s="20">
         <v>50000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J5" s="30"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>30</v>
       </c>
@@ -1082,8 +1098,9 @@
       <c r="I6" s="20">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J6" s="30"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>29</v>
       </c>
@@ -1111,8 +1128,9 @@
       <c r="I7" s="20">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="30"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>31</v>
       </c>
@@ -1140,8 +1158,9 @@
       <c r="I8" s="20">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>32</v>
       </c>
@@ -1169,8 +1188,9 @@
       <c r="I9" s="20">
         <v>500000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>33</v>
       </c>
@@ -1198,23 +1218,24 @@
       <c r="I10" s="20">
         <v>100000000</v>
       </c>
+      <c r="J10" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,37 +1244,39 @@
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="8" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1281,8 +1304,11 @@
       <c r="I3" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>26</v>
       </c>
@@ -1310,8 +1336,9 @@
       <c r="I4" s="12">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>35</v>
       </c>
@@ -1339,8 +1366,9 @@
       <c r="I5" s="12">
         <v>500000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1350,8 +1378,9 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -1361,8 +1390,9 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1372,8 +1402,9 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1383,14 +1414,15 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SphereTest input generation now working
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp45674\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1C24ED-8738-450F-9AF1-C27D6A00018C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0C9D9F-C0D4-4B67-98DA-3F74B3C29E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -243,7 +243,7 @@
     <t>/home/sbradnam/Projects/EPSRC/Benchmarking/software/freia/JADE/Configuration/openmc_config.sh</t>
   </si>
   <si>
-    <t>Custom Inputs</t>
+    <t>Custom Input</t>
   </si>
 </sst>
 </file>
@@ -477,6 +477,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,12 +499,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -828,10 +828,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,32 +951,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1038,7 +1038,7 @@
       <c r="I4" s="20">
         <v>10000000</v>
       </c>
-      <c r="J4" s="30"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -1068,7 +1068,7 @@
       <c r="I5" s="20">
         <v>50000000</v>
       </c>
-      <c r="J5" s="30"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -1098,7 +1098,7 @@
       <c r="I6" s="20">
         <v>10000000</v>
       </c>
-      <c r="J6" s="30"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
@@ -1128,7 +1128,7 @@
       <c r="I7" s="20">
         <v>10000000</v>
       </c>
-      <c r="J7" s="30"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
@@ -1158,7 +1158,7 @@
       <c r="I8" s="20">
         <v>100000000</v>
       </c>
-      <c r="J8" s="30"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -1188,7 +1188,7 @@
       <c r="I9" s="20">
         <v>500000000</v>
       </c>
-      <c r="J9" s="30"/>
+      <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
@@ -1218,7 +1218,7 @@
       <c r="I10" s="20">
         <v>100000000</v>
       </c>
-      <c r="J10" s="30"/>
+      <c r="J10" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1234,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,32 +1249,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -1336,7 +1336,7 @@
       <c r="I4" s="12">
         <v>10000000</v>
       </c>
-      <c r="J4" s="31"/>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1366,7 +1366,7 @@
       <c r="I5" s="12">
         <v>500000000</v>
       </c>
-      <c r="J5" s="31"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>

</xml_diff>

<commit_message>
SphereTests now running in terminal
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp45674\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp18501\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0C9D9F-C0D4-4B67-98DA-3F74B3C29E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFD3261-34AF-4E21-A63C-FE279C62B731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
@@ -818,7 +818,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +902,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="23">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,9 +1036,11 @@
         <v>21</v>
       </c>
       <c r="I4" s="20">
-        <v>10000000</v>
-      </c>
-      <c r="J4" s="24"/>
+        <v>1000000</v>
+      </c>
+      <c r="J4" s="24">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -1051,7 +1053,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>22</v>
@@ -1081,7 +1083,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>22</v>
@@ -1111,7 +1113,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>22</v>
@@ -1235,7 +1237,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1321,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>22</v>
@@ -1431,7 +1433,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added default code config.sh files, paths defined relative to Config.xlsx
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp18501\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp39738\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFD3261-34AF-4E21-A63C-FE279C62B731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24246FE-E7DF-46C8-996F-8E20024F3075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
   <si>
     <t>Default Benchmarks</t>
   </si>
@@ -180,12 +180,6 @@
     <t>/home/mcnp/mcnpexecs/freia/mcnp6v2_ifort2020_openmpi4.1_220706</t>
   </si>
   <si>
-    <t>/home/sbradnam/Projects/EPSRC/Benchmarking/software/freia/JADE/Configuration/mcnp_config.sh</t>
-  </si>
-  <si>
-    <t>/home/sbradnam/Software/freia/OPENMC_031122/openmc/build/bin/openmc</t>
-  </si>
-  <si>
     <t>Folder Name</t>
   </si>
   <si>
@@ -240,10 +234,22 @@
     <t>/home/mcnp/xs/xsdir_mcnp6.2_endfb8</t>
   </si>
   <si>
-    <t>/home/sbradnam/Projects/EPSRC/Benchmarking/software/freia/JADE/Configuration/openmc_config.sh</t>
-  </si>
-  <si>
     <t>Custom Input</t>
+  </si>
+  <si>
+    <t>openmc_config.sh</t>
+  </si>
+  <si>
+    <t>mcnp_config.sh</t>
+  </si>
+  <si>
+    <t>serpent_config.sh</t>
+  </si>
+  <si>
+    <t>/home/sbradnam/Software/freia/Serpent2_src/v2.1.32_ccfe/sss2</t>
+  </si>
+  <si>
+    <t>/home/sbradnam/Software/freia/OPENMC_311022/openmc/build/bin/openmc</t>
   </si>
 </sst>
 </file>
@@ -818,7 +824,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,27 +852,31 @@
         <v>38</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -874,18 +884,17 @@
         <v>42</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="23"/>
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="23"/>
     </row>
@@ -934,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,22 +992,22 @@
         <v>18</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="H3" s="17" t="s">
         <v>2</v>
@@ -1007,7 +1016,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1015,16 +1024,16 @@
         <v>19</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>22</v>
@@ -1047,7 +1056,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>22</v>
@@ -1077,7 +1086,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>22</v>
@@ -1107,7 +1116,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>22</v>
@@ -1137,7 +1146,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>22</v>
@@ -1167,7 +1176,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>22</v>
@@ -1197,7 +1206,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>22</v>
@@ -1283,22 +1292,22 @@
         <v>18</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>2</v>
@@ -1307,7 +1316,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1432,15 +1441,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F03233-EAF0-4262-AA38-EF4B945A3E70}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="64.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1455,16 +1464,16 @@
         <v>14</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1477,6 +1486,9 @@
       <c r="D2" t="s">
         <v>36</v>
       </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
       <c r="G2" t="s">
         <v>36</v>
       </c>
@@ -1489,10 +1501,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1503,10 +1518,13 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1517,10 +1535,13 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1533,6 +1554,9 @@
       <c r="D6" t="s">
         <v>36</v>
       </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" t="s">
         <v>36</v>
       </c>
@@ -1548,10 +1572,13 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated serpent xsdir paths
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp39738\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24246FE-E7DF-46C8-996F-8E20024F3075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78D7063-9DA4-4D05-9110-CBF78385CC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>Default Benchmarks</t>
   </si>
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>/home/sbradnam/Software/freia/OPENMC_311022/openmc/build/bin/openmc</t>
+  </si>
+  <si>
+    <t>/home/mcnp/xs/xsdir_mcnp6.2.serp</t>
+  </si>
+  <si>
+    <t>/home/mcnp/xs/xsdir_mcnp6.2_old.serp</t>
+  </si>
+  <si>
+    <t>/home/mcnp/xs/xsdir_mcnp6.2_jeff33_endfb71_fendl32b_irdff105_tt.serp</t>
+  </si>
+  <si>
+    <t>/home/mcnp/xs/xsdir_mcnp6.2_fendl32b_rw.serp</t>
+  </si>
+  <si>
+    <t>/home/mcnp/xs/xsdir_mcnp6.2_endfb8.serp</t>
   </si>
 </sst>
 </file>
@@ -1442,7 +1457,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1502,7 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
         <v>36</v>
@@ -1504,7 +1519,7 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
         <v>66</v>
@@ -1521,7 +1536,7 @@
         <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
         <v>64</v>
@@ -1538,7 +1553,7 @@
         <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
         <v>65</v>
@@ -1555,7 +1570,7 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
@@ -1575,7 +1590,7 @@
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Added openmc material generator, generates sphere tests
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp39738\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp37055\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78D7063-9DA4-4D05-9110-CBF78385CC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B100EDBF-3F99-49FA-86DC-2A4A494BF8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -839,7 +839,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,6 +906,7 @@
       <c r="A8" s="22" t="s">
         <v>62</v>
       </c>
+      <c r="B8" s="23"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
@@ -958,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1052,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>22</v>
@@ -1456,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F03233-EAF0-4262-AA38-EF4B945A3E70}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
OpenMC running plus job submission
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318EBD8E-762C-4E74-A735-9BAD96505191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D0A97F-2B74-4E73-8B36-EE39DD51F59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2595" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="5100" yWindow="2595" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
   <si>
     <t>Default Benchmarks</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>llsubmit</t>
+  </si>
+  <si>
+    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/fendl-3.1d-hdf5/cross_sections.xml</t>
+  </si>
+  <si>
+    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/endfb80_hdf5/cross_sections.xml</t>
   </si>
 </sst>
 </file>
@@ -435,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -512,6 +518,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E4" activeCellId="1" sqref="D4 E4"/>
     </sheetView>
   </sheetViews>
@@ -1447,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F03233-EAF0-4262-AA38-EF4B945A3E70}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,6 +1463,7 @@
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
     <col min="4" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.28515625" customWidth="1"/>
     <col min="7" max="7" width="64.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1495,6 +1503,7 @@
       <c r="E2" t="s">
         <v>72</v>
       </c>
+      <c r="F2" s="28"/>
       <c r="G2" t="s">
         <v>36</v>
       </c>
@@ -1512,6 +1521,7 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
+      <c r="F3" s="28"/>
       <c r="G3" t="s">
         <v>64</v>
       </c>
@@ -1529,6 +1539,9 @@
       <c r="E4" t="s">
         <v>74</v>
       </c>
+      <c r="F4" s="28" t="s">
+        <v>79</v>
+      </c>
       <c r="G4" t="s">
         <v>62</v>
       </c>
@@ -1546,6 +1559,7 @@
       <c r="E5" t="s">
         <v>75</v>
       </c>
+      <c r="F5" s="28"/>
       <c r="G5" t="s">
         <v>63</v>
       </c>
@@ -1563,6 +1577,7 @@
       <c r="E6" t="s">
         <v>72</v>
       </c>
+      <c r="F6" s="28"/>
       <c r="G6" t="s">
         <v>36</v>
       </c>
@@ -1582,6 +1597,9 @@
       </c>
       <c r="E7" t="s">
         <v>76</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>80</v>
       </c>
       <c r="G7" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Fixed job submission, serpent threading bug, auto user determination
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp46182\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE_V2\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D0A97F-2B74-4E73-8B36-EE39DD51F59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2712686B-35BF-4AF9-8B15-CD0E7D925AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2595" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -261,16 +261,16 @@
     <t>/home/mcnp/xs/xsdir_mcnp6.2_endfb8.serp</t>
   </si>
   <si>
+    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/fendl-3.1d-hdf5/cross_sections.xml</t>
+  </si>
+  <si>
+    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/endfb80_hdf5/cross_sections.xml</t>
+  </si>
+  <si>
+    <t>llsubmit</t>
+  </si>
+  <si>
     <t>Job_Script_Templates/LLtemplate.cmd</t>
-  </si>
-  <si>
-    <t>llsubmit</t>
-  </si>
-  <si>
-    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/fendl-3.1d-hdf5/cross_sections.xml</t>
-  </si>
-  <si>
-    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/endfb80_hdf5/cross_sections.xml</t>
   </si>
 </sst>
 </file>
@@ -500,6 +500,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,7 +519,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,7 +825,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1A2DE-3EB8-4AD4-9CF1-023800AFF144}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,10 +846,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -924,7 +924,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="21">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -932,7 +932,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -940,7 +940,7 @@
         <v>46</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -957,7 +957,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" activeCellId="1" sqref="D4 E4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,32 +973,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -1043,10 +1043,10 @@
         <v>22</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>21</v>
@@ -1061,7 +1061,7 @@
         <v>10000</v>
       </c>
       <c r="J4" s="17">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1273,32 +1273,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1454,7 +1454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F03233-EAF0-4262-AA38-EF4B945A3E70}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1503,7 +1503,7 @@
       <c r="E2" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="28"/>
+      <c r="F2" s="22"/>
       <c r="G2" t="s">
         <v>36</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="22"/>
       <c r="G3" t="s">
         <v>64</v>
       </c>
@@ -1539,8 +1539,8 @@
       <c r="E4" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>79</v>
+      <c r="F4" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="G4" t="s">
         <v>62</v>
@@ -1559,7 +1559,7 @@
       <c r="E5" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="22"/>
       <c r="G5" t="s">
         <v>63</v>
       </c>
@@ -1577,7 +1577,7 @@
       <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="22"/>
       <c r="G6" t="s">
         <v>36</v>
       </c>
@@ -1598,8 +1598,8 @@
       <c r="E7" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="28" t="s">
-        <v>80</v>
+      <c r="F7" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="G7" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Fixed initialisation bug with Isotopes.txt
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp46182\home\sbradnam\Projects\EPSRC\Benchmarking\software\freia\JADE_V2\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp02812\home\sbradnam\Projects\EPSRC\Benchmarking\software\drake\JADE\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2712686B-35BF-4AF9-8B15-CD0E7D925AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AFF795-C623-4470-8DE1-D8F7B55D55B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     <t>Batch file</t>
   </si>
   <si>
-    <t>/home/mcnp/mcnpexecs/freia/mcnp6v2_ifort2020_openmpi4.1_220706</t>
-  </si>
-  <si>
     <t>Folder Name</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>/home/sbradnam/Software/freia/Serpent2_src/v2.1.32_ccfe/sss2</t>
   </si>
   <si>
-    <t>/home/sbradnam/Software/freia/OPENMC_311022/openmc/build/bin/openmc</t>
-  </si>
-  <si>
     <t>/home/mcnp/xs/xsdir_mcnp6.2.serp</t>
   </si>
   <si>
@@ -261,16 +255,22 @@
     <t>/home/mcnp/xs/xsdir_mcnp6.2_endfb8.serp</t>
   </si>
   <si>
-    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/fendl-3.1d-hdf5/cross_sections.xml</t>
-  </si>
-  <si>
-    <t>/common/CUMULUS-TEMP/home/NEUTRONS/openmc/data/endfb80_hdf5/cross_sections.xml</t>
-  </si>
-  <si>
-    <t>llsubmit</t>
-  </si>
-  <si>
-    <t>Job_Script_Templates/LLtemplate.cmd</t>
+    <t>/home/sbradnam/Software/drake/DAG_OPENMC_021222/openmc/build/bin/openmc</t>
+  </si>
+  <si>
+    <t>/home/mcnp/mcnpexecs/drake/mcnp6v2_ifort2018_n1s</t>
+  </si>
+  <si>
+    <t>/home/sbradnam/Software/NEUTRONS/openmc/data/fendl-3.1d-hdf5/cross_sections.xml</t>
+  </si>
+  <si>
+    <t>/home/sbradnam/Software/NEUTRONS/openmc/data/endfb80_hdf5/cross_sections.xml</t>
+  </si>
+  <si>
+    <t>sbatch</t>
+  </si>
+  <si>
+    <t>Job_Script_Templates/Slurmtemplate.sh</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -864,7 +864,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -872,7 +872,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -880,7 +880,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -888,7 +888,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -896,18 +896,18 @@
         <v>42</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="21"/>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="21"/>
     </row>
@@ -924,7 +924,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="21">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -957,7 +957,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,22 +1005,22 @@
         <v>18</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>2</v>
@@ -1029,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>22</v>
@@ -1069,7 +1069,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>22</v>
@@ -1099,7 +1099,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>22</v>
@@ -1129,7 +1129,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>22</v>
@@ -1159,7 +1159,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>22</v>
@@ -1189,7 +1189,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>22</v>
@@ -1219,7 +1219,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>22</v>
@@ -1305,22 +1305,22 @@
         <v>18</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>2</v>
@@ -1329,7 +1329,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1454,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F03233-EAF0-4262-AA38-EF4B945A3E70}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,16 +1478,16 @@
         <v>14</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1501,7 +1501,7 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" t="s">
@@ -1516,14 +1516,14 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1534,16 +1534,16 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1554,14 +1554,14 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" t="s">
@@ -1593,16 +1593,16 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>